<commit_message>
changes to 1-get_osm_street_data and 2-update_activities
Added 'geosphere' package to 2-update_activities.
For 1-get_osm_street_data, added an additional filter to remove streets from df_progress file when flagged to remove (currently only removed partial streets)
</commit_message>
<xml_diff>
--- a/Data/manual_changes.xlsx
+++ b/Data/manual_changes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\haink\Documents\GitHub\RunEveryStreet\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BAC870D-1DDA-4977-8B26-A949DE16324C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EED86D7-97D6-4A86-83CE-A366549EBA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3576" yWindow="1848" windowWidth="15324" windowHeight="9720" tabRatio="729" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7776" yWindow="1800" windowWidth="15324" windowHeight="9720" tabRatio="729" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="osm_updates" sheetId="5" r:id="rId1"/>
@@ -22,12 +22,25 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">manual_completions!$A$1:$B$1</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4853" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4855" uniqueCount="102">
   <si>
     <t>osm_id</t>
   </si>
@@ -330,6 +343,9 @@
   </si>
   <si>
     <t>6th St</t>
+  </si>
+  <si>
+    <t>Windcrest Drive</t>
   </si>
 </sst>
 </file>
@@ -33766,10 +33782,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C102"/>
+  <dimension ref="A1:C103"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="B104" sqref="B104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -34816,6 +34832,17 @@
         <v>100</v>
       </c>
     </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <v>35165205</v>
+      </c>
+      <c r="B103" t="s">
+        <v>8</v>
+      </c>
+      <c r="C103" t="s">
+        <v>101</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -34824,10 +34851,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:A75"/>
+  <dimension ref="A1:A76"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A80" sqref="A80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35208,6 +35235,11 @@
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75">
         <v>48569778</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <v>966063205</v>
       </c>
     </row>
   </sheetData>
@@ -35567,10 +35599,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBB86B6D-07E8-4E85-B5C2-D754B644E697}">
-  <dimension ref="A1:D278"/>
+  <dimension ref="A1:D280"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A264" workbookViewId="0">
-      <selection activeCell="A277" sqref="A277"/>
+    <sheetView tabSelected="1" topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="D281" sqref="D281"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -39471,6 +39503,34 @@
       </c>
       <c r="D278">
         <v>21</v>
+      </c>
+    </row>
+    <row r="279" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A279">
+        <v>816658046</v>
+      </c>
+      <c r="B279" s="1">
+        <v>45243</v>
+      </c>
+      <c r="C279">
+        <v>2</v>
+      </c>
+      <c r="D279">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="280" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A280">
+        <v>35165205</v>
+      </c>
+      <c r="B280" s="1">
+        <v>45243</v>
+      </c>
+      <c r="C280">
+        <v>1</v>
+      </c>
+      <c r="D280">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>